<commit_message>
Vision por computador y otras asignaturas
</commit_message>
<xml_diff>
--- a/1º Cuatrimestre/Horario .xlsx
+++ b/1º Cuatrimestre/Horario .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidadhuelva-my.sharepoint.com/personal/alberto_fernandez320_alu_uhu_es/Documents/4º Curso/1º Cuatrimestre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="293" documentId="13_ncr:1_{950EE43C-9AA7-4A8F-8F41-62AF41A0D106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19D77D71-F365-44C2-899B-1E530643162F}"/>
+  <xr:revisionPtr revIDLastSave="295" documentId="13_ncr:1_{950EE43C-9AA7-4A8F-8F41-62AF41A0D106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1CC748B-6E2B-431C-9D71-E8DBB5DCA060}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>Días/Horas</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Procesamiento del habla, visión e interacción multimodal (ETP104)</t>
   </si>
   <si>
-    <t>Visión por Computador (PQ-110 Aula 1-4)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Visión por Computador  (GG2.11) </t>
   </si>
   <si>
@@ -157,6 +154,12 @@
   </si>
   <si>
     <t>Aprendizaje Automático (IM1.5)</t>
+  </si>
+  <si>
+    <t>Visión por Computador (IM1.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visión por Computador  (IM1.3) </t>
   </si>
 </sst>
 </file>
@@ -539,45 +542,118 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -585,79 +661,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -883,7 +886,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="H11" sqref="H11:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -895,80 +898,80 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="28" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="26" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="28" t="s">
+      <c r="G1" s="61"/>
+      <c r="H1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="24" t="s">
+      <c r="I1" s="57"/>
+      <c r="J1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="25"/>
+      <c r="K1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="29" t="s">
+      <c r="B2" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="31"/>
+      <c r="F2" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="31"/>
+      <c r="H2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="36"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="63"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="43"/>
       <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="38"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="43"/>
       <c r="L4" s="23"/>
       <c r="M4" s="8"/>
     </row>
@@ -976,148 +979,148 @@
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="29" t="s">
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="38"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="43"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="38"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="43"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="38"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="43"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="29" t="s">
+      <c r="B8" s="46"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="29" t="s">
+      <c r="G8" s="31"/>
+      <c r="H8" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="31"/>
+      <c r="J8" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="30"/>
-      <c r="J8" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" s="47"/>
+      <c r="K8" s="49"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="49"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="51"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="51"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="53"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="29" t="s">
+      <c r="B11" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="30"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="31"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="32"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="34"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1145,8 +1148,8 @@
       <c r="E15" s="18"/>
       <c r="F15" s="19"/>
       <c r="G15" s="17"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="36"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="63"/>
       <c r="J15" s="17"/>
       <c r="K15" s="18"/>
     </row>
@@ -1160,8 +1163,8 @@
       <c r="E16" s="18"/>
       <c r="F16" s="19"/>
       <c r="G16" s="17"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="43"/>
       <c r="J16" s="17"/>
       <c r="K16" s="18"/>
     </row>
@@ -1169,20 +1172,20 @@
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="54" t="s">
+      <c r="B17" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="55"/>
-      <c r="F17" s="60" t="s">
+      <c r="E17" s="25"/>
+      <c r="F17" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="61"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="38"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="43"/>
       <c r="J17" s="17"/>
       <c r="K17" s="18"/>
     </row>
@@ -1190,12 +1193,12 @@
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="63"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="39"/>
       <c r="H18" s="19"/>
       <c r="I18" s="18"/>
       <c r="J18" s="19"/>
@@ -1205,12 +1208,12 @@
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="65"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="41"/>
       <c r="H19" s="19"/>
       <c r="I19" s="18"/>
       <c r="J19" s="19"/>
@@ -1224,10 +1227,10 @@
       <c r="C20" s="18"/>
       <c r="D20" s="19"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="55"/>
+      <c r="F20" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="25"/>
       <c r="H20" s="19"/>
       <c r="I20" s="18"/>
       <c r="J20" s="19"/>
@@ -1241,8 +1244,8 @@
       <c r="C21" s="18"/>
       <c r="D21" s="19"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="57"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="19"/>
       <c r="I21" s="18"/>
       <c r="J21" s="19"/>
@@ -1256,8 +1259,8 @@
       <c r="C22" s="18"/>
       <c r="D22" s="19"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="59"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
       <c r="H22" s="19"/>
       <c r="I22" s="18"/>
       <c r="J22" s="19"/>
@@ -1271,10 +1274,10 @@
       <c r="C23" s="18"/>
       <c r="D23" s="19"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="54" t="s">
+      <c r="F23" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="55"/>
+      <c r="G23" s="25"/>
       <c r="H23" s="19"/>
       <c r="I23" s="18"/>
       <c r="J23" s="19"/>
@@ -1288,8 +1291,8 @@
       <c r="C24" s="18"/>
       <c r="D24" s="19"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="57"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
       <c r="H24" s="19"/>
       <c r="I24" s="18"/>
       <c r="J24" s="19"/>
@@ -1303,8 +1306,8 @@
       <c r="C25" s="21"/>
       <c r="D25" s="22"/>
       <c r="E25" s="21"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="59"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="29"/>
       <c r="H25" s="22"/>
       <c r="I25" s="21"/>
       <c r="J25" s="22"/>
@@ -2299,41 +2302,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="F20:G22"/>
-    <mergeCell ref="B17:C19"/>
-    <mergeCell ref="J11:K13"/>
-    <mergeCell ref="D17:E19"/>
-    <mergeCell ref="F23:G25"/>
-    <mergeCell ref="F17:G19"/>
-    <mergeCell ref="H8:I10"/>
-    <mergeCell ref="F8:G10"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B2:C4"/>
-    <mergeCell ref="D2:E4"/>
-    <mergeCell ref="F2:G4"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D5:E7"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
@@ -2350,6 +2318,41 @@
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D5:E7"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B2:C4"/>
+    <mergeCell ref="D2:E4"/>
+    <mergeCell ref="F2:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H8:I10"/>
+    <mergeCell ref="F8:G10"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F20:G22"/>
+    <mergeCell ref="B17:C19"/>
+    <mergeCell ref="J11:K13"/>
+    <mergeCell ref="D17:E19"/>
+    <mergeCell ref="F23:G25"/>
+    <mergeCell ref="F17:G19"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>